<commit_message>
Updated Access Log Reports
</commit_message>
<xml_diff>
--- a/Attendance(SulajAcharya)/April_Attendance(SulajAcharya).xlsx
+++ b/Attendance(SulajAcharya)/April_Attendance(SulajAcharya).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SulajAcharya\Godrej\Attendance(SulajAcharya)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E580993-6318-4B16-92D8-054A645A1034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621DD39D-4CE7-4B10-976E-34D1854777B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>TEAM ATTENDANCE - APRIL 2025</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Holiday for Ambedkar Jayanti</t>
   </si>
 </sst>
 </file>
@@ -519,12 +525,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -544,6 +544,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -763,13 +769,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X982"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="21.109375" customWidth="1"/>
+    <col min="1" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
@@ -780,11 +787,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.4">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -808,11 +815,11 @@
       <c r="X1" s="4"/>
     </row>
     <row r="2" spans="1:24" ht="14.4">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -839,10 +846,10 @@
       <c r="A3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="54"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -998,10 +1005,10 @@
       <c r="A9" s="43">
         <v>45753</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="48"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="21"/>
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
@@ -1208,10 +1215,10 @@
       <c r="A16" s="43">
         <v>45760</v>
       </c>
-      <c r="B16" s="44" t="s">
-        <v>3</v>
+      <c r="B16" s="54" t="s">
+        <v>4</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="28"/>
       <c r="E16" s="26"/>
       <c r="F16" s="4"/>
@@ -1239,9 +1246,11 @@
         <v>45761</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
-      <c r="C17" s="44"/>
+      <c r="C17" s="44" t="s">
+        <v>7</v>
+      </c>
       <c r="D17" s="28"/>
       <c r="E17" s="26"/>
       <c r="F17" s="4"/>
@@ -1388,9 +1397,7 @@
       <c r="A22" s="43">
         <v>45766</v>
       </c>
-      <c r="B22" s="44" t="s">
-        <v>3</v>
-      </c>
+      <c r="B22" s="44"/>
       <c r="C22" s="44"/>
       <c r="D22" s="31"/>
       <c r="E22" s="26"/>
@@ -1418,10 +1425,10 @@
       <c r="A23" s="43">
         <v>45767</v>
       </c>
-      <c r="B23" s="44" t="s">
-        <v>3</v>
+      <c r="B23" s="54" t="s">
+        <v>4</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="29"/>
       <c r="E23" s="26"/>
       <c r="F23" s="8"/>
@@ -1448,9 +1455,7 @@
       <c r="A24" s="43">
         <v>45768</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>3</v>
-      </c>
+      <c r="B24" s="44"/>
       <c r="C24" s="44"/>
       <c r="D24" s="31"/>
       <c r="E24" s="26"/>
@@ -1478,9 +1483,7 @@
       <c r="A25" s="43">
         <v>45769</v>
       </c>
-      <c r="B25" s="44" t="s">
-        <v>3</v>
-      </c>
+      <c r="B25" s="44"/>
       <c r="C25" s="45"/>
       <c r="D25" s="29"/>
       <c r="E25" s="26"/>
@@ -1508,9 +1511,7 @@
       <c r="A26" s="43">
         <v>45770</v>
       </c>
-      <c r="B26" s="44" t="s">
-        <v>3</v>
-      </c>
+      <c r="B26" s="44"/>
       <c r="C26" s="45"/>
       <c r="D26" s="31"/>
       <c r="E26" s="26"/>
@@ -1538,9 +1539,7 @@
       <c r="A27" s="43">
         <v>45771</v>
       </c>
-      <c r="B27" s="44" t="s">
-        <v>3</v>
-      </c>
+      <c r="B27" s="44"/>
       <c r="C27" s="45"/>
       <c r="D27" s="31"/>
       <c r="E27" s="26"/>
@@ -1628,10 +1627,10 @@
       <c r="A30" s="43">
         <v>45774</v>
       </c>
-      <c r="B30" s="44" t="s">
-        <v>3</v>
+      <c r="B30" s="54" t="s">
+        <v>4</v>
       </c>
-      <c r="C30" s="45"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="31"/>
       <c r="E30" s="26"/>
       <c r="F30" s="32"/>
@@ -26419,11 +26418,14 @@
       <c r="X982" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>